<commit_message>
Support CellAddress and default WidthPx, HeightPx
</commit_message>
<xml_diff>
--- a/samples/xlsx/TestIssue186_Template.xlsx
+++ b/samples/xlsx/TestIssue186_Template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\MiniExcel\samples\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9C0B66-EB09-416C-B622-D4E441399840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917CD811-34B3-44D9-A80B-A39A14EA2C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Demo" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -351,7 +351,7 @@
   <dimension ref="B3:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>